<commit_message>
Add DisplayFormat attribute to ExcelDynamicColumn
</commit_message>
<xml_diff>
--- a/ExcelReporter.Tests/TestData/DataSourceDynamicPanelDataReaderRenderTest/TestRenderDataReader.xlsx
+++ b/ExcelReporter.Tests/TestData/DataSourceDynamicPanelDataReaderRenderTest/TestRenderDataReader.xlsx
@@ -55,7 +55,7 @@
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="2">
     <x:numFmt numFmtId="0" formatCode=""/>
-    <x:numFmt numFmtId="165" formatCode="$ #,##0.00"/>
+    <x:numFmt numFmtId="165" formatCode="#,0.00"/>
   </x:numFmts>
   <x:fonts count="2">
     <x:font>
@@ -152,7 +152,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="4">
+  <x:cellStyleXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -162,11 +162,17 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="165" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="4">
+  <x:cellXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -179,7 +185,15 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -478,13 +492,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:R6"/>
+  <x:dimension ref="A1:Q6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="2" spans="1:18">
+    <x:row r="2" spans="1:17">
       <x:c r="B2" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -504,7 +518,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:18">
+    <x:row r="3" spans="1:17">
       <x:c r="B3" s="2" t="n">
         <x:v>1</x:v>
       </x:c>
@@ -516,11 +530,11 @@
       </x:c>
       <x:c r="E3" s="2" t="s"/>
       <x:c r="F3" s="2" t="s"/>
-      <x:c r="G3" s="2" t="n">
+      <x:c r="G3" s="3" t="n">
         <x:v>523635.93</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:18">
+    <x:row r="4" spans="1:17">
       <x:c r="B4" s="2" t="n">
         <x:v>2</x:v>
       </x:c>
@@ -536,9 +550,9 @@
       <x:c r="F4" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="G4" s="2" t="s"/>
+      <x:c r="G4" s="3" t="s"/>
     </x:row>
-    <x:row r="5" spans="1:18">
+    <x:row r="5" spans="1:17">
       <x:c r="B5" s="2" t="n">
         <x:v>3</x:v>
       </x:c>
@@ -550,17 +564,17 @@
       <x:c r="F5" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="G5" s="2" t="n">
+      <x:c r="G5" s="3" t="n">
         <x:v>100000.5532</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:18">
-      <x:c r="B6" s="3" t="s"/>
-      <x:c r="C6" s="3" t="s"/>
-      <x:c r="D6" s="3" t="s"/>
-      <x:c r="E6" s="3" t="s"/>
-      <x:c r="F6" s="3" t="s"/>
-      <x:c r="G6" s="3" t="n">
+    <x:row r="6" spans="1:17">
+      <x:c r="B6" s="5" t="s"/>
+      <x:c r="C6" s="5" t="s"/>
+      <x:c r="D6" s="5" t="s"/>
+      <x:c r="E6" s="5" t="s"/>
+      <x:c r="F6" s="5" t="s"/>
+      <x:c r="G6" s="4" t="n">
         <x:v>623636.4832</x:v>
       </x:c>
     </x:row>

</xml_diff>